<commit_message>
MLP for max return simulations
</commit_message>
<xml_diff>
--- a/experiments/pg/return_discount_increment/max_rew_mlp_3x182_corr_entropy_inp_time_step_3e_4_no_norm/oracle_buffer.xlsx
+++ b/experiments/pg/return_discount_increment/max_rew_mlp_3x182_corr_entropy_inp_time_step_3e_4_no_norm/oracle_buffer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2846"/>
+  <dimension ref="A1:C2962"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37430,6 +37430,1514 @@
         <v>14.57568870086847</v>
       </c>
     </row>
+    <row r="2847">
+      <c r="A2847" s="1" t="n">
+        <v>2845</v>
+      </c>
+      <c r="B2847" t="inlineStr">
+        <is>
+          <t>[5, 7, 1]</t>
+        </is>
+      </c>
+      <c r="C2847" t="n">
+        <v>14.31783948692184</v>
+      </c>
+    </row>
+    <row r="2848">
+      <c r="A2848" s="1" t="n">
+        <v>2846</v>
+      </c>
+      <c r="B2848" t="inlineStr">
+        <is>
+          <t>[3, 7, -1]</t>
+        </is>
+      </c>
+      <c r="C2848" t="n">
+        <v>15.46640714152086</v>
+      </c>
+    </row>
+    <row r="2849">
+      <c r="A2849" s="1" t="n">
+        <v>2847</v>
+      </c>
+      <c r="B2849" t="inlineStr">
+        <is>
+          <t>[4, 7, -1]</t>
+        </is>
+      </c>
+      <c r="C2849" t="n">
+        <v>14.23819195953667</v>
+      </c>
+    </row>
+    <row r="2850">
+      <c r="A2850" s="1" t="n">
+        <v>2848</v>
+      </c>
+      <c r="B2850" t="inlineStr">
+        <is>
+          <t>[4, 6, -1]</t>
+        </is>
+      </c>
+      <c r="C2850" t="n">
+        <v>14.43626685515152</v>
+      </c>
+    </row>
+    <row r="2851">
+      <c r="A2851" s="1" t="n">
+        <v>2849</v>
+      </c>
+      <c r="B2851" t="inlineStr">
+        <is>
+          <t>[4, 5, -1]</t>
+        </is>
+      </c>
+      <c r="C2851" t="n">
+        <v>14.55910845429896</v>
+      </c>
+    </row>
+    <row r="2852">
+      <c r="A2852" s="1" t="n">
+        <v>2850</v>
+      </c>
+      <c r="B2852" t="inlineStr">
+        <is>
+          <t>[3, 7, -2]</t>
+        </is>
+      </c>
+      <c r="C2852" t="n">
+        <v>14.43950852788879</v>
+      </c>
+    </row>
+    <row r="2853">
+      <c r="A2853" s="1" t="n">
+        <v>2851</v>
+      </c>
+      <c r="B2853" t="inlineStr">
+        <is>
+          <t>[3, 6, -2]</t>
+        </is>
+      </c>
+      <c r="C2853" t="n">
+        <v>14.49239652788212</v>
+      </c>
+    </row>
+    <row r="2854">
+      <c r="A2854" s="1" t="n">
+        <v>2852</v>
+      </c>
+      <c r="B2854" t="inlineStr">
+        <is>
+          <t>[5, 7, 0]</t>
+        </is>
+      </c>
+      <c r="C2854" t="n">
+        <v>14.2916524203408</v>
+      </c>
+    </row>
+    <row r="2855">
+      <c r="A2855" s="1" t="n">
+        <v>2853</v>
+      </c>
+      <c r="B2855" t="inlineStr">
+        <is>
+          <t>[2, 7, -2]</t>
+        </is>
+      </c>
+      <c r="C2855" t="n">
+        <v>15.47987207481578</v>
+      </c>
+    </row>
+    <row r="2856">
+      <c r="A2856" s="1" t="n">
+        <v>2854</v>
+      </c>
+      <c r="B2856" t="inlineStr">
+        <is>
+          <t>[6, 7, 1]</t>
+        </is>
+      </c>
+      <c r="C2856" t="n">
+        <v>14.47009555946217</v>
+      </c>
+    </row>
+    <row r="2857">
+      <c r="A2857" s="1" t="n">
+        <v>2855</v>
+      </c>
+      <c r="B2857" t="inlineStr">
+        <is>
+          <t>[6, 7, 0]</t>
+        </is>
+      </c>
+      <c r="C2857" t="n">
+        <v>14.68923399264573</v>
+      </c>
+    </row>
+    <row r="2858">
+      <c r="A2858" s="1" t="n">
+        <v>2856</v>
+      </c>
+      <c r="B2858" t="inlineStr">
+        <is>
+          <t>[4, 6, -2]</t>
+        </is>
+      </c>
+      <c r="C2858" t="n">
+        <v>14.09966332258864</v>
+      </c>
+    </row>
+    <row r="2859">
+      <c r="A2859" s="1" t="n">
+        <v>2857</v>
+      </c>
+      <c r="B2859" t="inlineStr">
+        <is>
+          <t>[3, 6, -3]</t>
+        </is>
+      </c>
+      <c r="C2859" t="n">
+        <v>14.23435105657102</v>
+      </c>
+    </row>
+    <row r="2860">
+      <c r="A2860" s="1" t="n">
+        <v>2858</v>
+      </c>
+      <c r="B2860" t="inlineStr">
+        <is>
+          <t>[3, 5, -3]</t>
+        </is>
+      </c>
+      <c r="C2860" t="n">
+        <v>14.33962475007306</v>
+      </c>
+    </row>
+    <row r="2861">
+      <c r="A2861" s="1" t="n">
+        <v>2859</v>
+      </c>
+      <c r="B2861" t="inlineStr">
+        <is>
+          <t>[5, 7, -1]</t>
+        </is>
+      </c>
+      <c r="C2861" t="n">
+        <v>14.2063651533609</v>
+      </c>
+    </row>
+    <row r="2862">
+      <c r="A2862" s="1" t="n">
+        <v>2860</v>
+      </c>
+      <c r="B2862" t="inlineStr">
+        <is>
+          <t>[7, 7, 1]</t>
+        </is>
+      </c>
+      <c r="C2862" t="n">
+        <v>14.57550314259325</v>
+      </c>
+    </row>
+    <row r="2863">
+      <c r="A2863" s="1" t="n">
+        <v>2861</v>
+      </c>
+      <c r="B2863" t="inlineStr">
+        <is>
+          <t>[5, 6, -1]</t>
+        </is>
+      </c>
+      <c r="C2863" t="n">
+        <v>14.2358144428755</v>
+      </c>
+    </row>
+    <row r="2864">
+      <c r="A2864" s="1" t="n">
+        <v>2862</v>
+      </c>
+      <c r="B2864" t="inlineStr">
+        <is>
+          <t>[4, 7, -2]</t>
+        </is>
+      </c>
+      <c r="C2864" t="n">
+        <v>14.03743089434232</v>
+      </c>
+    </row>
+    <row r="2865">
+      <c r="A2865" s="1" t="n">
+        <v>2863</v>
+      </c>
+      <c r="B2865" t="inlineStr">
+        <is>
+          <t>[4, 5, -2]</t>
+        </is>
+      </c>
+      <c r="C2865" t="n">
+        <v>14.15908284862589</v>
+      </c>
+    </row>
+    <row r="2866">
+      <c r="A2866" s="1" t="n">
+        <v>2864</v>
+      </c>
+      <c r="B2866" t="inlineStr">
+        <is>
+          <t>[7, 6, 1]</t>
+        </is>
+      </c>
+      <c r="C2866" t="n">
+        <v>14.61960251297191</v>
+      </c>
+    </row>
+    <row r="2867">
+      <c r="A2867" s="1" t="n">
+        <v>2865</v>
+      </c>
+      <c r="B2867" t="inlineStr">
+        <is>
+          <t>[6, 6, 0]</t>
+        </is>
+      </c>
+      <c r="C2867" t="n">
+        <v>14.67113684352342</v>
+      </c>
+    </row>
+    <row r="2868">
+      <c r="A2868" s="1" t="n">
+        <v>2866</v>
+      </c>
+      <c r="B2868" t="inlineStr">
+        <is>
+          <t>[5, 5, -1]</t>
+        </is>
+      </c>
+      <c r="C2868" t="n">
+        <v>14.12758809177826</v>
+      </c>
+    </row>
+    <row r="2869">
+      <c r="A2869" s="1" t="n">
+        <v>2867</v>
+      </c>
+      <c r="B2869" t="inlineStr">
+        <is>
+          <t>[6, 7, -1]</t>
+        </is>
+      </c>
+      <c r="C2869" t="n">
+        <v>14.37562758978605</v>
+      </c>
+    </row>
+    <row r="2870">
+      <c r="A2870" s="1" t="n">
+        <v>2868</v>
+      </c>
+      <c r="B2870" t="inlineStr">
+        <is>
+          <t>[4, 5, -3]</t>
+        </is>
+      </c>
+      <c r="C2870" t="n">
+        <v>14.0677783305574</v>
+      </c>
+    </row>
+    <row r="2871">
+      <c r="A2871" s="1" t="n">
+        <v>2869</v>
+      </c>
+      <c r="B2871" t="inlineStr">
+        <is>
+          <t>[6, 5, 0]</t>
+        </is>
+      </c>
+      <c r="C2871" t="n">
+        <v>14.87328792327715</v>
+      </c>
+    </row>
+    <row r="2872">
+      <c r="A2872" s="1" t="n">
+        <v>2870</v>
+      </c>
+      <c r="B2872" t="inlineStr">
+        <is>
+          <t>[5, 7, -2]</t>
+        </is>
+      </c>
+      <c r="C2872" t="n">
+        <v>14.0195287816899</v>
+      </c>
+    </row>
+    <row r="2873">
+      <c r="A2873" s="1" t="n">
+        <v>2871</v>
+      </c>
+      <c r="B2873" t="inlineStr">
+        <is>
+          <t>[4, 7, -3]</t>
+        </is>
+      </c>
+      <c r="C2873" t="n">
+        <v>13.99555079167001</v>
+      </c>
+    </row>
+    <row r="2874">
+      <c r="A2874" s="1" t="n">
+        <v>2872</v>
+      </c>
+      <c r="B2874" t="inlineStr">
+        <is>
+          <t>[3, 7, -3]</t>
+        </is>
+      </c>
+      <c r="C2874" t="n">
+        <v>14.21189433701692</v>
+      </c>
+    </row>
+    <row r="2875">
+      <c r="A2875" s="1" t="n">
+        <v>2873</v>
+      </c>
+      <c r="B2875" t="inlineStr">
+        <is>
+          <t>[7, 7, 0]</t>
+        </is>
+      </c>
+      <c r="C2875" t="n">
+        <v>14.74326922826796</v>
+      </c>
+    </row>
+    <row r="2876">
+      <c r="A2876" s="1" t="n">
+        <v>2874</v>
+      </c>
+      <c r="B2876" t="inlineStr">
+        <is>
+          <t>[4, 6, -3]</t>
+        </is>
+      </c>
+      <c r="C2876" t="n">
+        <v>14.03164526768943</v>
+      </c>
+    </row>
+    <row r="2877">
+      <c r="A2877" s="1" t="n">
+        <v>2875</v>
+      </c>
+      <c r="B2877" t="inlineStr">
+        <is>
+          <t>[6, 6, -1]</t>
+        </is>
+      </c>
+      <c r="C2877" t="n">
+        <v>14.35119955658427</v>
+      </c>
+    </row>
+    <row r="2878">
+      <c r="A2878" s="1" t="n">
+        <v>2876</v>
+      </c>
+      <c r="B2878" t="inlineStr">
+        <is>
+          <t>[5, 6, -2]</t>
+        </is>
+      </c>
+      <c r="C2878" t="n">
+        <v>14.02759029358675</v>
+      </c>
+    </row>
+    <row r="2879">
+      <c r="A2879" s="1" t="n">
+        <v>2877</v>
+      </c>
+      <c r="B2879" t="inlineStr">
+        <is>
+          <t>[7, 6, 0]</t>
+        </is>
+      </c>
+      <c r="C2879" t="n">
+        <v>14.76768720552464</v>
+      </c>
+    </row>
+    <row r="2880">
+      <c r="A2880" s="1" t="n">
+        <v>2878</v>
+      </c>
+      <c r="B2880" t="inlineStr">
+        <is>
+          <t>[6, 5, -1]</t>
+        </is>
+      </c>
+      <c r="C2880" t="n">
+        <v>14.49867151118834</v>
+      </c>
+    </row>
+    <row r="2881">
+      <c r="A2881" s="1" t="n">
+        <v>2879</v>
+      </c>
+      <c r="B2881" t="inlineStr">
+        <is>
+          <t>[7, 5, 1]</t>
+        </is>
+      </c>
+      <c r="C2881" t="n">
+        <v>14.68425410164483</v>
+      </c>
+    </row>
+    <row r="2882">
+      <c r="A2882" s="1" t="n">
+        <v>2880</v>
+      </c>
+      <c r="B2882" t="inlineStr">
+        <is>
+          <t>[5, 5, -2]</t>
+        </is>
+      </c>
+      <c r="C2882" t="n">
+        <v>13.98439257472053</v>
+      </c>
+    </row>
+    <row r="2883">
+      <c r="A2883" s="1" t="n">
+        <v>2881</v>
+      </c>
+      <c r="B2883" t="inlineStr">
+        <is>
+          <t>[7, 7, -1]</t>
+        </is>
+      </c>
+      <c r="C2883" t="n">
+        <v>14.32693469241859</v>
+      </c>
+    </row>
+    <row r="2884">
+      <c r="A2884" s="1" t="n">
+        <v>2882</v>
+      </c>
+      <c r="B2884" t="inlineStr">
+        <is>
+          <t>[6, 6, -2]</t>
+        </is>
+      </c>
+      <c r="C2884" t="n">
+        <v>14.06640745994208</v>
+      </c>
+    </row>
+    <row r="2885">
+      <c r="A2885" s="1" t="n">
+        <v>2883</v>
+      </c>
+      <c r="B2885" t="inlineStr">
+        <is>
+          <t>[6, 5, -2]</t>
+        </is>
+      </c>
+      <c r="C2885" t="n">
+        <v>14.11943469131286</v>
+      </c>
+    </row>
+    <row r="2886">
+      <c r="A2886" s="1" t="n">
+        <v>2884</v>
+      </c>
+      <c r="B2886" t="inlineStr">
+        <is>
+          <t>[7, 5, 0]</t>
+        </is>
+      </c>
+      <c r="C2886" t="n">
+        <v>14.80224424922126</v>
+      </c>
+    </row>
+    <row r="2887">
+      <c r="A2887" s="1" t="n">
+        <v>2885</v>
+      </c>
+      <c r="B2887" t="inlineStr">
+        <is>
+          <t>[7, 4, 1]</t>
+        </is>
+      </c>
+      <c r="C2887" t="n">
+        <v>14.87403651387894</v>
+      </c>
+    </row>
+    <row r="2888">
+      <c r="A2888" s="1" t="n">
+        <v>2886</v>
+      </c>
+      <c r="B2888" t="inlineStr">
+        <is>
+          <t>[6, 7, -2]</t>
+        </is>
+      </c>
+      <c r="C2888" t="n">
+        <v>14.07790118406906</v>
+      </c>
+    </row>
+    <row r="2889">
+      <c r="A2889" s="1" t="n">
+        <v>2887</v>
+      </c>
+      <c r="B2889" t="inlineStr">
+        <is>
+          <t>[7, 6, -1]</t>
+        </is>
+      </c>
+      <c r="C2889" t="n">
+        <v>14.3665454117861</v>
+      </c>
+    </row>
+    <row r="2890">
+      <c r="A2890" s="1" t="n">
+        <v>2888</v>
+      </c>
+      <c r="B2890" t="inlineStr">
+        <is>
+          <t>[7, 7, -2]</t>
+        </is>
+      </c>
+      <c r="C2890" t="n">
+        <v>14.05723684906032</v>
+      </c>
+    </row>
+    <row r="2891">
+      <c r="A2891" s="1" t="n">
+        <v>2889</v>
+      </c>
+      <c r="B2891" t="inlineStr">
+        <is>
+          <t>[7, 6, -2]</t>
+        </is>
+      </c>
+      <c r="C2891" t="n">
+        <v>14.06975517639637</v>
+      </c>
+    </row>
+    <row r="2892">
+      <c r="A2892" s="1" t="n">
+        <v>2890</v>
+      </c>
+      <c r="B2892" t="inlineStr">
+        <is>
+          <t>[7, 5, -1]</t>
+        </is>
+      </c>
+      <c r="C2892" t="n">
+        <v>14.39589684679759</v>
+      </c>
+    </row>
+    <row r="2893">
+      <c r="A2893" s="1" t="n">
+        <v>2891</v>
+      </c>
+      <c r="B2893" t="inlineStr">
+        <is>
+          <t>[7, 3, 1]</t>
+        </is>
+      </c>
+      <c r="C2893" t="n">
+        <v>14.97396957050487</v>
+      </c>
+    </row>
+    <row r="2894">
+      <c r="A2894" s="1" t="n">
+        <v>2892</v>
+      </c>
+      <c r="B2894" t="inlineStr">
+        <is>
+          <t>[7, 5, -2]</t>
+        </is>
+      </c>
+      <c r="C2894" t="n">
+        <v>14.08245932389138</v>
+      </c>
+    </row>
+    <row r="2895">
+      <c r="A2895" s="1" t="n">
+        <v>2893</v>
+      </c>
+      <c r="B2895" t="inlineStr">
+        <is>
+          <t>[6, 4, -2]</t>
+        </is>
+      </c>
+      <c r="C2895" t="n">
+        <v>14.20489214364643</v>
+      </c>
+    </row>
+    <row r="2896">
+      <c r="A2896" s="1" t="n">
+        <v>2894</v>
+      </c>
+      <c r="B2896" t="inlineStr">
+        <is>
+          <t>[7, 4, 0]</t>
+        </is>
+      </c>
+      <c r="C2896" t="n">
+        <v>14.86678394046673</v>
+      </c>
+    </row>
+    <row r="2897">
+      <c r="A2897" s="1" t="n">
+        <v>2895</v>
+      </c>
+      <c r="B2897" t="inlineStr">
+        <is>
+          <t>[7, 4, -1]</t>
+        </is>
+      </c>
+      <c r="C2897" t="n">
+        <v>14.42846118163782</v>
+      </c>
+    </row>
+    <row r="2898">
+      <c r="A2898" s="1" t="n">
+        <v>2896</v>
+      </c>
+      <c r="B2898" t="inlineStr">
+        <is>
+          <t>[5, 5, -3]</t>
+        </is>
+      </c>
+      <c r="C2898" t="n">
+        <v>13.95896677329353</v>
+      </c>
+    </row>
+    <row r="2899">
+      <c r="A2899" s="1" t="n">
+        <v>2897</v>
+      </c>
+      <c r="B2899" t="inlineStr">
+        <is>
+          <t>[7, 3, 0]</t>
+        </is>
+      </c>
+      <c r="C2899" t="n">
+        <v>14.80450291699727</v>
+      </c>
+    </row>
+    <row r="2900">
+      <c r="A2900" s="1" t="n">
+        <v>2898</v>
+      </c>
+      <c r="B2900" t="inlineStr">
+        <is>
+          <t>[7, 4, -2]</t>
+        </is>
+      </c>
+      <c r="C2900" t="n">
+        <v>14.10594468937919</v>
+      </c>
+    </row>
+    <row r="2901">
+      <c r="A2901" s="1" t="n">
+        <v>2899</v>
+      </c>
+      <c r="B2901" t="inlineStr">
+        <is>
+          <t>[7, 3, -2]</t>
+        </is>
+      </c>
+      <c r="C2901" t="n">
+        <v>14.08158525971881</v>
+      </c>
+    </row>
+    <row r="2902">
+      <c r="A2902" s="1" t="n">
+        <v>2900</v>
+      </c>
+      <c r="B2902" t="inlineStr">
+        <is>
+          <t>[6, 2, 0]</t>
+        </is>
+      </c>
+      <c r="C2902" t="n">
+        <v>14.8309644498828</v>
+      </c>
+    </row>
+    <row r="2903">
+      <c r="A2903" s="1" t="n">
+        <v>2901</v>
+      </c>
+      <c r="B2903" t="inlineStr">
+        <is>
+          <t>[7, 2, 2]</t>
+        </is>
+      </c>
+      <c r="C2903" t="n">
+        <v>14.13984075572462</v>
+      </c>
+    </row>
+    <row r="2904">
+      <c r="A2904" s="1" t="n">
+        <v>2902</v>
+      </c>
+      <c r="B2904" t="inlineStr">
+        <is>
+          <t>[7, 3, -1]</t>
+        </is>
+      </c>
+      <c r="C2904" t="n">
+        <v>14.35411352994062</v>
+      </c>
+    </row>
+    <row r="2905">
+      <c r="A2905" s="1" t="n">
+        <v>2903</v>
+      </c>
+      <c r="B2905" t="inlineStr">
+        <is>
+          <t>[7, 2, -1]</t>
+        </is>
+      </c>
+      <c r="C2905" t="n">
+        <v>14.48206661456856</v>
+      </c>
+    </row>
+    <row r="2906">
+      <c r="A2906" s="1" t="n">
+        <v>2904</v>
+      </c>
+      <c r="B2906" t="inlineStr">
+        <is>
+          <t>[6, 2, -1]</t>
+        </is>
+      </c>
+      <c r="C2906" t="n">
+        <v>14.48049039517381</v>
+      </c>
+    </row>
+    <row r="2907">
+      <c r="A2907" s="1" t="n">
+        <v>2905</v>
+      </c>
+      <c r="B2907" t="inlineStr">
+        <is>
+          <t>[7, 2, 0]</t>
+        </is>
+      </c>
+      <c r="C2907" t="n">
+        <v>14.75369558145824</v>
+      </c>
+    </row>
+    <row r="2908">
+      <c r="A2908" s="1" t="n">
+        <v>2906</v>
+      </c>
+      <c r="B2908" t="inlineStr">
+        <is>
+          <t>[7, 1, 2]</t>
+        </is>
+      </c>
+      <c r="C2908" t="n">
+        <v>14.93359506218911</v>
+      </c>
+    </row>
+    <row r="2909">
+      <c r="A2909" s="1" t="n">
+        <v>2907</v>
+      </c>
+      <c r="B2909" t="inlineStr">
+        <is>
+          <t>[6, 1, 0]</t>
+        </is>
+      </c>
+      <c r="C2909" t="n">
+        <v>14.71194613131143</v>
+      </c>
+    </row>
+    <row r="2910">
+      <c r="A2910" s="1" t="n">
+        <v>2908</v>
+      </c>
+      <c r="B2910" t="inlineStr">
+        <is>
+          <t>[6, 1, -1]</t>
+        </is>
+      </c>
+      <c r="C2910" t="n">
+        <v>14.56521747655457</v>
+      </c>
+    </row>
+    <row r="2911">
+      <c r="A2911" s="1" t="n">
+        <v>2909</v>
+      </c>
+      <c r="B2911" t="inlineStr">
+        <is>
+          <t>[7, 1, 0]</t>
+        </is>
+      </c>
+      <c r="C2911" t="n">
+        <v>14.7533782592117</v>
+      </c>
+    </row>
+    <row r="2912">
+      <c r="A2912" s="1" t="n">
+        <v>2910</v>
+      </c>
+      <c r="B2912" t="inlineStr">
+        <is>
+          <t>[6, 0, 0]</t>
+        </is>
+      </c>
+      <c r="C2912" t="n">
+        <v>14.65563985356643</v>
+      </c>
+    </row>
+    <row r="2913">
+      <c r="A2913" s="1" t="n">
+        <v>2911</v>
+      </c>
+      <c r="B2913" t="inlineStr">
+        <is>
+          <t>[7, 0, 1]</t>
+        </is>
+      </c>
+      <c r="C2913" t="n">
+        <v>14.7533782620727</v>
+      </c>
+    </row>
+    <row r="2914">
+      <c r="A2914" s="1" t="n">
+        <v>2912</v>
+      </c>
+      <c r="B2914" t="inlineStr">
+        <is>
+          <t>[7, 0, 2]</t>
+        </is>
+      </c>
+      <c r="C2914" t="n">
+        <v>14.75369558168724</v>
+      </c>
+    </row>
+    <row r="2915">
+      <c r="A2915" s="1" t="n">
+        <v>2913</v>
+      </c>
+      <c r="B2915" t="inlineStr">
+        <is>
+          <t>[6, -1, 2]</t>
+        </is>
+      </c>
+      <c r="C2915" t="n">
+        <v>14.48049039522741</v>
+      </c>
+    </row>
+    <row r="2916">
+      <c r="A2916" s="1" t="n">
+        <v>2914</v>
+      </c>
+      <c r="B2916" t="inlineStr">
+        <is>
+          <t>[7, 0, 0]</t>
+        </is>
+      </c>
+      <c r="C2916" t="n">
+        <v>14.73125241134602</v>
+      </c>
+    </row>
+    <row r="2917">
+      <c r="A2917" s="1" t="n">
+        <v>2915</v>
+      </c>
+      <c r="B2917" t="inlineStr">
+        <is>
+          <t>[7, -1, 2]</t>
+        </is>
+      </c>
+      <c r="C2917" t="n">
+        <v>14.48206661438547</v>
+      </c>
+    </row>
+    <row r="2918">
+      <c r="A2918" s="1" t="n">
+        <v>2916</v>
+      </c>
+      <c r="B2918" t="inlineStr">
+        <is>
+          <t>[7, -1, 1]</t>
+        </is>
+      </c>
+      <c r="C2918" t="n">
+        <v>14.6821893785849</v>
+      </c>
+    </row>
+    <row r="2919">
+      <c r="A2919" s="1" t="n">
+        <v>2917</v>
+      </c>
+      <c r="B2919" t="inlineStr">
+        <is>
+          <t>[6, 0, -1]</t>
+        </is>
+      </c>
+      <c r="C2919" t="n">
+        <v>14.68393866534542</v>
+      </c>
+    </row>
+    <row r="2920">
+      <c r="A2920" s="1" t="n">
+        <v>2918</v>
+      </c>
+      <c r="B2920" t="inlineStr">
+        <is>
+          <t>[6, -1, 0]</t>
+        </is>
+      </c>
+      <c r="C2920" t="n">
+        <v>14.68393866281813</v>
+      </c>
+    </row>
+    <row r="2921">
+      <c r="A2921" s="1" t="n">
+        <v>2919</v>
+      </c>
+      <c r="B2921" t="inlineStr">
+        <is>
+          <t>[7, -2, 2]</t>
+        </is>
+      </c>
+      <c r="C2921" t="n">
+        <v>14.21739224578428</v>
+      </c>
+    </row>
+    <row r="2922">
+      <c r="A2922" s="1" t="n">
+        <v>2920</v>
+      </c>
+      <c r="B2922" t="inlineStr">
+        <is>
+          <t>[6, -2, 1]</t>
+        </is>
+      </c>
+      <c r="C2922" t="n">
+        <v>14.44603305727835</v>
+      </c>
+    </row>
+    <row r="2923">
+      <c r="A2923" s="1" t="n">
+        <v>2921</v>
+      </c>
+      <c r="B2923" t="inlineStr">
+        <is>
+          <t>[6, -2, 0]</t>
+        </is>
+      </c>
+      <c r="C2923" t="n">
+        <v>14.69680375717896</v>
+      </c>
+    </row>
+    <row r="2924">
+      <c r="A2924" s="1" t="n">
+        <v>2922</v>
+      </c>
+      <c r="B2924" t="inlineStr">
+        <is>
+          <t>[7, -2, 1]</t>
+        </is>
+      </c>
+      <c r="C2924" t="n">
+        <v>14.61417565491659</v>
+      </c>
+    </row>
+    <row r="2925">
+      <c r="A2925" s="1" t="n">
+        <v>2923</v>
+      </c>
+      <c r="B2925" t="inlineStr">
+        <is>
+          <t>[6, -3, 1]</t>
+        </is>
+      </c>
+      <c r="C2925" t="n">
+        <v>14.37242159182118</v>
+      </c>
+    </row>
+    <row r="2926">
+      <c r="A2926" s="1" t="n">
+        <v>2924</v>
+      </c>
+      <c r="B2926" t="inlineStr">
+        <is>
+          <t>[7, -2, 0]</t>
+        </is>
+      </c>
+      <c r="C2926" t="n">
+        <v>14.82171046217402</v>
+      </c>
+    </row>
+    <row r="2927">
+      <c r="A2927" s="1" t="n">
+        <v>2925</v>
+      </c>
+      <c r="B2927" t="inlineStr">
+        <is>
+          <t>[7, -1, 0]</t>
+        </is>
+      </c>
+      <c r="C2927" t="n">
+        <v>14.81562667066004</v>
+      </c>
+    </row>
+    <row r="2928">
+      <c r="A2928" s="1" t="n">
+        <v>2926</v>
+      </c>
+      <c r="B2928" t="inlineStr">
+        <is>
+          <t>[7, -3, 0]</t>
+        </is>
+      </c>
+      <c r="C2928" t="n">
+        <v>14.7912476945207</v>
+      </c>
+    </row>
+    <row r="2929">
+      <c r="A2929" s="1" t="n">
+        <v>2927</v>
+      </c>
+      <c r="B2929" t="inlineStr">
+        <is>
+          <t>[7, -4, 0]</t>
+        </is>
+      </c>
+      <c r="C2929" t="n">
+        <v>14.75038705031406</v>
+      </c>
+    </row>
+    <row r="2930">
+      <c r="A2930" s="1" t="n">
+        <v>2928</v>
+      </c>
+      <c r="B2930" t="inlineStr">
+        <is>
+          <t>[7, -3, 1]</t>
+        </is>
+      </c>
+      <c r="C2930" t="n">
+        <v>14.57669807604962</v>
+      </c>
+    </row>
+    <row r="2931">
+      <c r="A2931" s="1" t="n">
+        <v>2929</v>
+      </c>
+      <c r="B2931" t="inlineStr">
+        <is>
+          <t>[7, -3, 2]</t>
+        </is>
+      </c>
+      <c r="C2931" t="n">
+        <v>14.14948773254473</v>
+      </c>
+    </row>
+    <row r="2932">
+      <c r="A2932" s="1" t="n">
+        <v>2930</v>
+      </c>
+      <c r="B2932" t="inlineStr">
+        <is>
+          <t>[6, -3, 0]</t>
+        </is>
+      </c>
+      <c r="C2932" t="n">
+        <v>14.68941130562881</v>
+      </c>
+    </row>
+    <row r="2933">
+      <c r="A2933" s="1" t="n">
+        <v>2931</v>
+      </c>
+      <c r="B2933" t="inlineStr">
+        <is>
+          <t>[7, -4, 1]</t>
+        </is>
+      </c>
+      <c r="C2933" t="n">
+        <v>14.57578656126839</v>
+      </c>
+    </row>
+    <row r="2934">
+      <c r="A2934" s="1" t="n">
+        <v>2932</v>
+      </c>
+      <c r="B2934" t="inlineStr">
+        <is>
+          <t>[6, -4, 1]</t>
+        </is>
+      </c>
+      <c r="C2934" t="n">
+        <v>14.36361946401663</v>
+      </c>
+    </row>
+    <row r="2935">
+      <c r="A2935" s="1" t="n">
+        <v>2933</v>
+      </c>
+      <c r="B2935" t="inlineStr">
+        <is>
+          <t>[6, -1, -1]</t>
+        </is>
+      </c>
+      <c r="C2935" t="n">
+        <v>14.34518346960254</v>
+      </c>
+    </row>
+    <row r="2936">
+      <c r="A2936" s="1" t="n">
+        <v>2934</v>
+      </c>
+      <c r="B2936" t="inlineStr">
+        <is>
+          <t>[7, -3, 3]</t>
+        </is>
+      </c>
+      <c r="C2936" t="n">
+        <v>14.00569635649737</v>
+      </c>
+    </row>
+    <row r="2937">
+      <c r="A2937" s="1" t="n">
+        <v>2935</v>
+      </c>
+      <c r="B2937" t="inlineStr">
+        <is>
+          <t>[7, 0, -1]</t>
+        </is>
+      </c>
+      <c r="C2937" t="n">
+        <v>14.81562666892938</v>
+      </c>
+    </row>
+    <row r="2938">
+      <c r="A2938" s="1" t="n">
+        <v>2936</v>
+      </c>
+      <c r="B2938" t="inlineStr">
+        <is>
+          <t>[7, -1, -1]</t>
+        </is>
+      </c>
+      <c r="C2938" t="n">
+        <v>14.32308696635742</v>
+      </c>
+    </row>
+    <row r="2939">
+      <c r="A2939" s="1" t="n">
+        <v>2937</v>
+      </c>
+      <c r="B2939" t="inlineStr">
+        <is>
+          <t>[7, -2, -1]</t>
+        </is>
+      </c>
+      <c r="C2939" t="n">
+        <v>14.7549035937702</v>
+      </c>
+    </row>
+    <row r="2940">
+      <c r="A2940" s="1" t="n">
+        <v>2938</v>
+      </c>
+      <c r="B2940" t="inlineStr">
+        <is>
+          <t>[7, 1, -1]</t>
+        </is>
+      </c>
+      <c r="C2940" t="n">
+        <v>14.68218937857749</v>
+      </c>
+    </row>
+    <row r="2941">
+      <c r="A2941" s="1" t="n">
+        <v>2939</v>
+      </c>
+      <c r="B2941" t="inlineStr">
+        <is>
+          <t>[7, 0, -2]</t>
+        </is>
+      </c>
+      <c r="C2941" t="n">
+        <v>14.82171046229748</v>
+      </c>
+    </row>
+    <row r="2942">
+      <c r="A2942" s="1" t="n">
+        <v>2940</v>
+      </c>
+      <c r="B2942" t="inlineStr">
+        <is>
+          <t>[7, -1, -2]</t>
+        </is>
+      </c>
+      <c r="C2942" t="n">
+        <v>14.7549036023258</v>
+      </c>
+    </row>
+    <row r="2943">
+      <c r="A2943" s="1" t="n">
+        <v>2941</v>
+      </c>
+      <c r="B2943" t="inlineStr">
+        <is>
+          <t>[6, 1, -2]</t>
+        </is>
+      </c>
+      <c r="C2943" t="n">
+        <v>14.44603305727735</v>
+      </c>
+    </row>
+    <row r="2944">
+      <c r="A2944" s="1" t="n">
+        <v>2942</v>
+      </c>
+      <c r="B2944" t="inlineStr">
+        <is>
+          <t>[7, 2, -2]</t>
+        </is>
+      </c>
+      <c r="C2944" t="n">
+        <v>14.2173922457169</v>
+      </c>
+    </row>
+    <row r="2945">
+      <c r="A2945" s="1" t="n">
+        <v>2943</v>
+      </c>
+      <c r="B2945" t="inlineStr">
+        <is>
+          <t>[7, 1, -2]</t>
+        </is>
+      </c>
+      <c r="C2945" t="n">
+        <v>14.6141756548483</v>
+      </c>
+    </row>
+    <row r="2946">
+      <c r="A2946" s="1" t="n">
+        <v>2944</v>
+      </c>
+      <c r="B2946" t="inlineStr">
+        <is>
+          <t>[6, 0, -2]</t>
+        </is>
+      </c>
+      <c r="C2946" t="n">
+        <v>14.69680375754639</v>
+      </c>
+    </row>
+    <row r="2947">
+      <c r="A2947" s="1" t="n">
+        <v>2945</v>
+      </c>
+      <c r="B2947" t="inlineStr">
+        <is>
+          <t>[6, 2, -2]</t>
+        </is>
+      </c>
+      <c r="C2947" t="n">
+        <v>14.179044659973</v>
+      </c>
+    </row>
+    <row r="2948">
+      <c r="A2948" s="1" t="n">
+        <v>2946</v>
+      </c>
+      <c r="B2948" t="inlineStr">
+        <is>
+          <t>[7, 3, -3]</t>
+        </is>
+      </c>
+      <c r="C2948" t="n">
+        <v>14.00569635642744</v>
+      </c>
+    </row>
+    <row r="2949">
+      <c r="A2949" s="1" t="n">
+        <v>2947</v>
+      </c>
+      <c r="B2949" t="inlineStr">
+        <is>
+          <t>[7, 2, -3]</t>
+        </is>
+      </c>
+      <c r="C2949" t="n">
+        <v>14.14948773270023</v>
+      </c>
+    </row>
+    <row r="2950">
+      <c r="A2950" s="1" t="n">
+        <v>2948</v>
+      </c>
+      <c r="B2950" t="inlineStr">
+        <is>
+          <t>[6, 2, -3]</t>
+        </is>
+      </c>
+      <c r="C2950" t="n">
+        <v>14.09710607144536</v>
+      </c>
+    </row>
+    <row r="2951">
+      <c r="A2951" s="1" t="n">
+        <v>2949</v>
+      </c>
+      <c r="B2951" t="inlineStr">
+        <is>
+          <t>[6, 1, -3]</t>
+        </is>
+      </c>
+      <c r="C2951" t="n">
+        <v>14.37242159191559</v>
+      </c>
+    </row>
+    <row r="2952">
+      <c r="A2952" s="1" t="n">
+        <v>2950</v>
+      </c>
+      <c r="B2952" t="inlineStr">
+        <is>
+          <t>[7, 6, -3]</t>
+        </is>
+      </c>
+      <c r="C2952" t="n">
+        <v>14.00404537862574</v>
+      </c>
+    </row>
+    <row r="2953">
+      <c r="A2953" s="1" t="n">
+        <v>2951</v>
+      </c>
+      <c r="B2953" t="inlineStr">
+        <is>
+          <t>[7, 5, -3]</t>
+        </is>
+      </c>
+      <c r="C2953" t="n">
+        <v>14.01421953625679</v>
+      </c>
+    </row>
+    <row r="2954">
+      <c r="A2954" s="1" t="n">
+        <v>2952</v>
+      </c>
+      <c r="B2954" t="inlineStr">
+        <is>
+          <t>[6, 5, -3]</t>
+        </is>
+      </c>
+      <c r="C2954" t="n">
+        <v>14.03451694536387</v>
+      </c>
+    </row>
+    <row r="2955">
+      <c r="A2955" s="1" t="n">
+        <v>2953</v>
+      </c>
+      <c r="B2955" t="inlineStr">
+        <is>
+          <t>[6, 4, -3]</t>
+        </is>
+      </c>
+      <c r="C2955" t="n">
+        <v>14.07331007835756</v>
+      </c>
+    </row>
+    <row r="2956">
+      <c r="A2956" s="1" t="n">
+        <v>2954</v>
+      </c>
+      <c r="B2956" t="inlineStr">
+        <is>
+          <t>[6, 3, -3]</t>
+        </is>
+      </c>
+      <c r="C2956" t="n">
+        <v>14.03284744428706</v>
+      </c>
+    </row>
+    <row r="2957">
+      <c r="A2957" s="1" t="n">
+        <v>2955</v>
+      </c>
+      <c r="B2957" t="inlineStr">
+        <is>
+          <t>[7, 4, -3]</t>
+        </is>
+      </c>
+      <c r="C2957" t="n">
+        <v>14.02323980749771</v>
+      </c>
+    </row>
+    <row r="2958">
+      <c r="A2958" s="1" t="n">
+        <v>2956</v>
+      </c>
+      <c r="B2958" t="inlineStr">
+        <is>
+          <t>[5, 4, -3]</t>
+        </is>
+      </c>
+      <c r="C2958" t="n">
+        <v>14.04434061232261</v>
+      </c>
+    </row>
+    <row r="2959">
+      <c r="A2959" s="1" t="n">
+        <v>2957</v>
+      </c>
+      <c r="B2959" t="inlineStr">
+        <is>
+          <t>[7, 7, -3]</t>
+        </is>
+      </c>
+      <c r="C2959" t="n">
+        <v>13.99627260743519</v>
+      </c>
+    </row>
+    <row r="2960">
+      <c r="A2960" s="1" t="n">
+        <v>2958</v>
+      </c>
+      <c r="B2960" t="inlineStr">
+        <is>
+          <t>[6, 6, -3]</t>
+        </is>
+      </c>
+      <c r="C2960" t="n">
+        <v>14.00161598525918</v>
+      </c>
+    </row>
+    <row r="2961">
+      <c r="A2961" s="1" t="n">
+        <v>2959</v>
+      </c>
+      <c r="B2961" t="inlineStr">
+        <is>
+          <t>[6, 7, -3]</t>
+        </is>
+      </c>
+      <c r="C2961" t="n">
+        <v>14.00999727919645</v>
+      </c>
+    </row>
+    <row r="2962">
+      <c r="A2962" s="1" t="n">
+        <v>2960</v>
+      </c>
+      <c r="B2962" t="inlineStr">
+        <is>
+          <t>[5, 6, -3]</t>
+        </is>
+      </c>
+      <c r="C2962" t="n">
+        <v>13.9850955318668</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>